<commit_message>
Completed Reliabilit y Metric
Completed Reliability Metric
</commit_message>
<xml_diff>
--- a/documents/Implementation/ImplementationMetrics.xlsx
+++ b/documents/Implementation/ImplementationMetrics.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency" sheetId="1" r:id="rId1"/>
     <sheet name="Reliability" sheetId="2" r:id="rId2"/>
-    <sheet name="Security" sheetId="3" r:id="rId3"/>
+    <sheet name="Robustness" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,11 +25,231 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+  <si>
+    <t>Robustness</t>
+  </si>
+  <si>
+    <t>Reliability</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>#144</t>
+  </si>
+  <si>
+    <t>Travis CI Failed Build #</t>
+  </si>
+  <si>
+    <t>#143</t>
+  </si>
+  <si>
+    <t>Time in seconds</t>
+  </si>
+  <si>
+    <t>#113</t>
+  </si>
+  <si>
+    <t>#112</t>
+  </si>
+  <si>
+    <t>#105</t>
+  </si>
+  <si>
+    <t>#103</t>
+  </si>
+  <si>
+    <t>#101</t>
+  </si>
+  <si>
+    <t>#100</t>
+  </si>
+  <si>
+    <t>#99</t>
+  </si>
+  <si>
+    <t>#98</t>
+  </si>
+  <si>
+    <t>#97</t>
+  </si>
+  <si>
+    <t>#96</t>
+  </si>
+  <si>
+    <t>#95</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>#13</t>
+  </si>
+  <si>
+    <t>#15</t>
+  </si>
+  <si>
+    <t>#16</t>
+  </si>
+  <si>
+    <t>#21</t>
+  </si>
+  <si>
+    <t>#22</t>
+  </si>
+  <si>
+    <t>#27</t>
+  </si>
+  <si>
+    <t>#28</t>
+  </si>
+  <si>
+    <t>#29</t>
+  </si>
+  <si>
+    <t>#31</t>
+  </si>
+  <si>
+    <t>#36</t>
+  </si>
+  <si>
+    <t>#37</t>
+  </si>
+  <si>
+    <t>#38</t>
+  </si>
+  <si>
+    <t>#39</t>
+  </si>
+  <si>
+    <t>#40</t>
+  </si>
+  <si>
+    <t>#41</t>
+  </si>
+  <si>
+    <t>#42</t>
+  </si>
+  <si>
+    <t>#43</t>
+  </si>
+  <si>
+    <t>#44</t>
+  </si>
+  <si>
+    <t>#45</t>
+  </si>
+  <si>
+    <t>#46</t>
+  </si>
+  <si>
+    <t>#47</t>
+  </si>
+  <si>
+    <t>#48</t>
+  </si>
+  <si>
+    <t>#49</t>
+  </si>
+  <si>
+    <t>#50</t>
+  </si>
+  <si>
+    <t>#51</t>
+  </si>
+  <si>
+    <t>#52</t>
+  </si>
+  <si>
+    <t>#53</t>
+  </si>
+  <si>
+    <t>#54</t>
+  </si>
+  <si>
+    <t>#55</t>
+  </si>
+  <si>
+    <t>#56</t>
+  </si>
+  <si>
+    <t>#57</t>
+  </si>
+  <si>
+    <t>#59</t>
+  </si>
+  <si>
+    <t>#64</t>
+  </si>
+  <si>
+    <t>#65</t>
+  </si>
+  <si>
+    <t>#66</t>
+  </si>
+  <si>
+    <t>#68</t>
+  </si>
+  <si>
+    <t>#69</t>
+  </si>
+  <si>
+    <t>Mean Time to Failure (seconds)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -56,8 +276,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,24 +608,579 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C3" s="1">
+        <v>42684</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="4">
+        <f>AVERAGE(B8:B69)</f>
+        <v>136.01612903225808</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="4">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="4">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="4">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="4">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="4">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="4">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="4">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="4">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="4">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="4">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="4">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="4">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="4">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="4">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="4">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="4">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="4">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="4">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="4">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" s="4">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="4">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="4">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" s="4">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" s="4">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>42684</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated reliability & robustness 11/16/2016
</commit_message>
<xml_diff>
--- a/documents/Implementation/ImplementationMetrics.xlsx
+++ b/documents/Implementation/ImplementationMetrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
   <si>
     <t>Robustness</t>
   </si>
@@ -287,13 +287,25 @@
   </si>
   <si>
     <t>1 / 1.1 KBytes</t>
+  </si>
+  <si>
+    <t>#176</t>
+  </si>
+  <si>
+    <t>#209</t>
+  </si>
+  <si>
+    <t>#225</t>
+  </si>
+  <si>
+    <t>43 / 52</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +350,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -365,13 +385,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,14 +724,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3"/>
-      <c r="C3" s="5">
+      <c r="C3" s="11">
         <v>42684</v>
       </c>
       <c r="D3"/>
@@ -720,30 +740,30 @@
       <c r="G3"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B6" t="s">
@@ -766,7 +786,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B7" t="s">
@@ -787,6 +807,9 @@
       <c r="G7" t="s">
         <v>83</v>
       </c>
+    </row>
+    <row r="10" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -796,10 +819,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,59 +831,98 @@
     <col min="2" max="2" width="16.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="30.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="C3" s="1">
         <v>42684</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="I3" s="1">
+        <v>42690</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="4">
+      <c r="G7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4">
+        <v>69</v>
+      </c>
+      <c r="D8" s="4">
         <f>AVERAGE(B8:B69)</f>
         <v>136.01612903225808</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8">
+        <v>47</v>
+      </c>
+      <c r="J8" s="4">
+        <f>AVERAGE(H8:H69)</f>
+        <v>249.66666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="4">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="4">
         <v>79</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -868,7 +930,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -876,7 +938,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -884,7 +946,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -892,7 +954,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -900,7 +962,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1339,41 +1401,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42684</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="D3" s="1">
+        <v>42690</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3">
         <v>0.71</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated implementation metrics. adding plugins back in to eslintrc
</commit_message>
<xml_diff>
--- a/documents/Implementation/ImplementationMetrics.xlsx
+++ b/documents/Implementation/ImplementationMetrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
   <si>
     <t>Robustness</t>
   </si>
@@ -323,6 +323,27 @@
   </si>
   <si>
     <t>1 / 166.7 B</t>
+  </si>
+  <si>
+    <t>15 / 28</t>
+  </si>
+  <si>
+    <t>#264</t>
+  </si>
+  <si>
+    <t>#266</t>
+  </si>
+  <si>
+    <t>#294</t>
+  </si>
+  <si>
+    <t>#296</t>
+  </si>
+  <si>
+    <t>#311</t>
+  </si>
+  <si>
+    <t>#321</t>
   </si>
 </sst>
 </file>
@@ -741,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -911,10 +932,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,22 +948,29 @@
     <col min="8" max="8" width="16.140625" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="10" max="10" width="30.7109375" customWidth="1"/>
+    <col min="12" max="12" width="24" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="C3" s="1">
         <v>42684</v>
       </c>
       <c r="I3" s="1">
         <v>42690</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N3" s="1">
+        <v>42695</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -963,8 +991,18 @@
       <c r="J7" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -985,8 +1023,18 @@
         <f>AVERAGE(H8:H69)</f>
         <v>249.66666666666666</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>105</v>
+      </c>
+      <c r="M8">
+        <v>176</v>
+      </c>
+      <c r="O8" s="4">
+        <f>AVERAGE(M8:M69)</f>
+        <v>159.16666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -999,8 +1047,14 @@
       <c r="H9">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1013,32 +1067,56 @@
       <c r="H10">
         <v>653</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>103</v>
+      </c>
+      <c r="M10">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="4">
         <v>94</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>102</v>
+      </c>
+      <c r="M11">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="4">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="4">
         <v>95</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>100</v>
+      </c>
+      <c r="M13">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1046,7 +1124,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1132,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1493,32 +1571,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>42684</v>
       </c>
       <c r="D3" s="1">
         <v>42690</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>42695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>67</v>
       </c>
@@ -1528,8 +1610,11 @@
       <c r="D5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
@@ -1538,6 +1623,9 @@
       </c>
       <c r="D6" s="3">
         <v>0.82</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated reliability & efficiency metrics
</commit_message>
<xml_diff>
--- a/documents/Implementation/ImplementationMetrics.xlsx
+++ b/documents/Implementation/ImplementationMetrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="142">
   <si>
     <t>Robustness</t>
   </si>
@@ -346,15 +346,6 @@
     <t>#321</t>
   </si>
   <si>
-    <t>There were not any</t>
-  </si>
-  <si>
-    <t>failed builds</t>
-  </si>
-  <si>
-    <t>since november 21</t>
-  </si>
-  <si>
     <t>12 / 13.2 KB</t>
   </si>
   <si>
@@ -380,6 +371,87 @@
   </si>
   <si>
     <t>1 / 63.42 B</t>
+  </si>
+  <si>
+    <t>42 / 2.7 KB</t>
+  </si>
+  <si>
+    <t>48 / 3.0 KB</t>
+  </si>
+  <si>
+    <t>49 / 1.8 KB</t>
+  </si>
+  <si>
+    <t>1 / 64.3 B</t>
+  </si>
+  <si>
+    <t>1 / 50 B</t>
+  </si>
+  <si>
+    <t>1 / 62.5 B</t>
+  </si>
+  <si>
+    <t>#446</t>
+  </si>
+  <si>
+    <t>#445</t>
+  </si>
+  <si>
+    <t>#443</t>
+  </si>
+  <si>
+    <t>#429</t>
+  </si>
+  <si>
+    <t>#424</t>
+  </si>
+  <si>
+    <t>#422</t>
+  </si>
+  <si>
+    <t>#420</t>
+  </si>
+  <si>
+    <t>#411</t>
+  </si>
+  <si>
+    <t>#400</t>
+  </si>
+  <si>
+    <t>#386</t>
+  </si>
+  <si>
+    <t>#385</t>
+  </si>
+  <si>
+    <t>#384</t>
+  </si>
+  <si>
+    <t>#382</t>
+  </si>
+  <si>
+    <t>#377</t>
+  </si>
+  <si>
+    <t>#378</t>
+  </si>
+  <si>
+    <t>#379</t>
+  </si>
+  <si>
+    <t>#380</t>
+  </si>
+  <si>
+    <t>#381</t>
+  </si>
+  <si>
+    <t>#375</t>
+  </si>
+  <si>
+    <t>#370</t>
+  </si>
+  <si>
+    <t>#359</t>
   </si>
 </sst>
 </file>
@@ -798,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,10 +1015,10 @@
         <v>96</v>
       </c>
       <c r="F13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -969,7 +1041,7 @@
         <v>92</v>
       </c>
       <c r="G14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -1005,22 +1077,22 @@
         <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" t="s">
         <v>116</v>
       </c>
-      <c r="D20" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F20" t="s">
-        <v>109</v>
-      </c>
       <c r="G20" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1028,10 +1100,22 @@
         <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>114</v>
+      </c>
+      <c r="D21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1044,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="M7" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,6 +1149,7 @@
     <col min="17" max="17" width="23.140625" customWidth="1"/>
     <col min="18" max="18" width="15.85546875" customWidth="1"/>
     <col min="19" max="19" width="21.28515625" customWidth="1"/>
+    <col min="20" max="20" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="23.25" x14ac:dyDescent="0.35">
@@ -1083,7 +1168,7 @@
         <v>42695</v>
       </c>
       <c r="S3" s="1">
-        <v>42698</v>
+        <v>42709</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1159,7 +1244,16 @@
         <f>AVERAGE(M8:M69)</f>
         <v>159.16666666666666</v>
       </c>
-      <c r="T8" s="4"/>
+      <c r="Q8" t="s">
+        <v>121</v>
+      </c>
+      <c r="R8">
+        <v>33</v>
+      </c>
+      <c r="T8" s="4">
+        <f>AVERAGE(R8:R28)</f>
+        <v>165.66666666666666</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1180,6 +1274,12 @@
       <c r="M9">
         <v>190</v>
       </c>
+      <c r="Q9" t="s">
+        <v>122</v>
+      </c>
+      <c r="R9">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1201,13 +1301,10 @@
         <v>177</v>
       </c>
       <c r="Q10" t="s">
-        <v>106</v>
-      </c>
-      <c r="R10" t="s">
-        <v>107</v>
-      </c>
-      <c r="S10" t="s">
-        <v>108</v>
+        <v>123</v>
+      </c>
+      <c r="R10">
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1223,6 +1320,12 @@
       <c r="M11">
         <v>182</v>
       </c>
+      <c r="Q11" t="s">
+        <v>124</v>
+      </c>
+      <c r="R11">
+        <v>202</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1237,6 +1340,12 @@
       <c r="M12">
         <v>124</v>
       </c>
+      <c r="Q12" t="s">
+        <v>125</v>
+      </c>
+      <c r="R12">
+        <v>164</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1251,6 +1360,12 @@
       <c r="M13">
         <v>106</v>
       </c>
+      <c r="Q13" t="s">
+        <v>126</v>
+      </c>
+      <c r="R13">
+        <v>163</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1259,6 +1374,12 @@
       <c r="B14" s="4">
         <v>104</v>
       </c>
+      <c r="Q14" t="s">
+        <v>127</v>
+      </c>
+      <c r="R14">
+        <v>156</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1267,6 +1388,12 @@
       <c r="B15" s="4">
         <v>78</v>
       </c>
+      <c r="Q15" t="s">
+        <v>128</v>
+      </c>
+      <c r="R15">
+        <v>178</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1275,104 +1402,182 @@
       <c r="B16" s="4">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>129</v>
+      </c>
+      <c r="R16">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="4">
         <v>112</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>130</v>
+      </c>
+      <c r="R17">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="4">
         <v>89</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>131</v>
+      </c>
+      <c r="R18">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="4">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>132</v>
+      </c>
+      <c r="R19">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="4">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q20" t="s">
+        <v>133</v>
+      </c>
+      <c r="R20">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="4">
         <v>82</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q21" t="s">
+        <v>138</v>
+      </c>
+      <c r="R21">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>65</v>
       </c>
       <c r="B22" s="4">
         <v>206</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q22" t="s">
+        <v>137</v>
+      </c>
+      <c r="R22">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
       <c r="B23" s="4">
         <v>185</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q23" t="s">
+        <v>136</v>
+      </c>
+      <c r="R23">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
       <c r="B24" s="4">
         <v>78</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>135</v>
+      </c>
+      <c r="R24">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>62</v>
       </c>
       <c r="B25" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>134</v>
+      </c>
+      <c r="R25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="4">
         <v>210</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>139</v>
+      </c>
+      <c r="R26">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>60</v>
       </c>
       <c r="B27" s="4">
         <v>195</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>140</v>
+      </c>
+      <c r="R27">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
       <c r="B28" s="4">
         <v>294</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="Q28" t="s">
+        <v>141</v>
+      </c>
+      <c r="R28">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -1380,7 +1585,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -1388,7 +1593,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -1396,7 +1601,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1784,10 +1989,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
eslint plugins back in
</commit_message>
<xml_diff>
--- a/documents/Implementation/ImplementationMetrics.xlsx
+++ b/documents/Implementation/ImplementationMetrics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Efficiency" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="142">
   <si>
     <t>Robustness</t>
   </si>
@@ -1128,7 +1128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M7" workbookViewId="0">
+    <sheetView topLeftCell="M7" workbookViewId="0">
       <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
@@ -1914,8 +1914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,6 +1986,9 @@
       <c r="F9" s="1">
         <v>42709</v>
       </c>
+      <c r="H9" s="1">
+        <v>42711</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
@@ -1994,12 +1997,18 @@
       <c r="F11" t="s">
         <v>110</v>
       </c>
+      <c r="H11" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="3">
         <v>0.56999999999999995</v>
       </c>
       <c r="F12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="3">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>